<commit_message>
replaced item in array with .includes
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\Desktop\web\analysis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8520F2-29D9-49B5-B878-7092A2540AE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
-    <sheet name="out" sheetId="1" r:id="rId1"/>
+    <sheet name="out" sheetId="2" r:id="rId1"/>
+    <sheet name="old_out" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -80,11 +75,131 @@
   <si>
     <t>Shift</t>
   </si>
+  <si>
+    <t>2020-11-29-00_52_42</t>
+  </si>
+  <si>
+    <t>2020-11-29-00_43_47</t>
+  </si>
+  <si>
+    <t>2020-11-29-21_47_27</t>
+  </si>
+  <si>
+    <t>2020-12-02-10_07_51</t>
+  </si>
+  <si>
+    <t>2020-12-02-14_47_37</t>
+  </si>
+  <si>
+    <t>2020-12-03-09_28_29</t>
+  </si>
+  <si>
+    <t>2020-11-03-12_56_57</t>
+  </si>
+  <si>
+    <t>2020-11-06-20_03_45</t>
+  </si>
+  <si>
+    <t>2020-11-07-14_32_58</t>
+  </si>
+  <si>
+    <t>2020-11-07-20_59_44</t>
+  </si>
+  <si>
+    <t>2020-11-08-20_39_35</t>
+  </si>
+  <si>
+    <t>2020-11-08-22_12_45</t>
+  </si>
+  <si>
+    <t>2020-11-08-22_38_18</t>
+  </si>
+  <si>
+    <t>2020-11-08-20_45_07</t>
+  </si>
+  <si>
+    <t>2020-11-08-21_09_32</t>
+  </si>
+  <si>
+    <t>2020-11-09-09_37_48</t>
+  </si>
+  <si>
+    <t>2020-11-09-17_23_37</t>
+  </si>
+  <si>
+    <t>2020-11-04-12_16_07</t>
+  </si>
+  <si>
+    <t>2020-11-06-11_57_01</t>
+  </si>
+  <si>
+    <t>2020-11-06-19_56_55</t>
+  </si>
+  <si>
+    <t>2020-11-11-08_52_51</t>
+  </si>
+  <si>
+    <t>2020-11-12-10_11_43</t>
+  </si>
+  <si>
+    <t>2020-11-14-16_39_14</t>
+  </si>
+  <si>
+    <t>2020-11-15-12_27_48</t>
+  </si>
+  <si>
+    <t>2020-11-18-10_18_10</t>
+  </si>
+  <si>
+    <t>2020-11-03-20_36_43</t>
+  </si>
+  <si>
+    <t>2020-11-04-19_04_10</t>
+  </si>
+  <si>
+    <t>2020-11-04-19_17_48</t>
+  </si>
+  <si>
+    <t>2020-11-13-11_32_26</t>
+  </si>
+  <si>
+    <t>2020-11-20-11_00_11</t>
+  </si>
+  <si>
+    <t>2020-11-25-09_39_16</t>
+  </si>
+  <si>
+    <t>2020-11-29-00_34_38</t>
+  </si>
+  <si>
+    <t>2020-11-16-01_57_42</t>
+  </si>
+  <si>
+    <t>2020-11-15-13_41_35</t>
+  </si>
+  <si>
+    <t>2020-11-19-09_56_11</t>
+  </si>
+  <si>
+    <t>2020-11-22-13_43_38</t>
+  </si>
+  <si>
+    <t>2020-11-23-11_03_27</t>
+  </si>
+  <si>
+    <t>2020-11-24-09_40_07</t>
+  </si>
+  <si>
+    <t>2020-11-27-16_13_13</t>
+  </si>
+  <si>
+    <t>55dc916737cc6e7fe2aad88af1a55e8517b3f86d2e5da0a95ced1b3a822cb6e7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
@@ -720,7 +835,87 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1063,17 +1258,3033 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>1268912</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>141</v>
+      </c>
+      <c r="E3">
+        <v>103600</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3">
+        <v>646895</v>
+      </c>
+      <c r="H3">
+        <v>0.50980288625215897</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>920465</v>
+      </c>
+      <c r="K3">
+        <v>0.725397033048785</v>
+      </c>
+      <c r="L3">
+        <v>14</v>
+      </c>
+      <c r="M3">
+        <v>1182242</v>
+      </c>
+      <c r="N3">
+        <v>0.93169739115084405</v>
+      </c>
+      <c r="O3">
+        <v>35</v>
+      </c>
+      <c r="P3">
+        <v>1234331</v>
+      </c>
+      <c r="Q3">
+        <v>0.97274751913450197</v>
+      </c>
+      <c r="R3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>1326448</v>
+      </c>
+      <c r="C4">
+        <f>B4-B3</f>
+        <v>57536</v>
+      </c>
+      <c r="D4">
+        <v>141</v>
+      </c>
+      <c r="E4">
+        <v>118408</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>684395</v>
+      </c>
+      <c r="H4">
+        <v>0.515960670904551</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>957965</v>
+      </c>
+      <c r="K4">
+        <v>0.72220320736282095</v>
+      </c>
+      <c r="L4">
+        <v>14</v>
+      </c>
+      <c r="M4">
+        <v>1237242</v>
+      </c>
+      <c r="N4">
+        <v>0.932748211765557</v>
+      </c>
+      <c r="O4">
+        <v>35</v>
+      </c>
+      <c r="P4">
+        <v>1291831</v>
+      </c>
+      <c r="Q4">
+        <v>0.97390248241921196</v>
+      </c>
+      <c r="R4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>1352868</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C41" si="0">B5-B4</f>
+        <v>26420</v>
+      </c>
+      <c r="D5">
+        <v>143</v>
+      </c>
+      <c r="E5">
+        <v>118908</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>684895</v>
+      </c>
+      <c r="H5">
+        <v>0.50625412087505905</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>976965</v>
+      </c>
+      <c r="K5">
+        <v>0.72214362376817198</v>
+      </c>
+      <c r="L5">
+        <v>14</v>
+      </c>
+      <c r="M5">
+        <v>1268571</v>
+      </c>
+      <c r="N5">
+        <v>0.93769015158906799</v>
+      </c>
+      <c r="O5">
+        <v>36</v>
+      </c>
+      <c r="P5">
+        <v>1319160</v>
+      </c>
+      <c r="Q5">
+        <v>0.97508404367610102</v>
+      </c>
+      <c r="R5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>1440842</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>87974</v>
+      </c>
+      <c r="D6">
+        <v>143</v>
+      </c>
+      <c r="E6">
+        <v>123908</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>694898</v>
+      </c>
+      <c r="H6">
+        <v>0.482286052183376</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>1042662</v>
+      </c>
+      <c r="K6">
+        <v>0.72364770044182503</v>
+      </c>
+      <c r="L6">
+        <v>14</v>
+      </c>
+      <c r="M6">
+        <v>1354768</v>
+      </c>
+      <c r="N6">
+        <v>0.94026131942294799</v>
+      </c>
+      <c r="O6">
+        <v>36</v>
+      </c>
+      <c r="P6">
+        <v>1407557</v>
+      </c>
+      <c r="Q6">
+        <v>0.97689892437893899</v>
+      </c>
+      <c r="R6">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7">
+        <v>1440845</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>143</v>
+      </c>
+      <c r="E7">
+        <v>123908</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>694898</v>
+      </c>
+      <c r="H7">
+        <v>0.48228504801002098</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>1042663</v>
+      </c>
+      <c r="K7">
+        <v>0.72364688776377695</v>
+      </c>
+      <c r="L7">
+        <v>14</v>
+      </c>
+      <c r="M7">
+        <v>1354769</v>
+      </c>
+      <c r="N7">
+        <v>0.94026005573118498</v>
+      </c>
+      <c r="O7">
+        <v>36</v>
+      </c>
+      <c r="P7">
+        <v>1407558</v>
+      </c>
+      <c r="Q7">
+        <v>0.97689758440359598</v>
+      </c>
+      <c r="R7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>1501904</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>61059</v>
+      </c>
+      <c r="D8">
+        <v>168</v>
+      </c>
+      <c r="E8">
+        <v>123908</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>776095</v>
+      </c>
+      <c r="H8">
+        <v>0.51674075040748202</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>1129562</v>
+      </c>
+      <c r="K8">
+        <v>0.75208668463496997</v>
+      </c>
+      <c r="L8">
+        <v>17</v>
+      </c>
+      <c r="M8">
+        <v>1422962</v>
+      </c>
+      <c r="N8">
+        <v>0.94743871778755495</v>
+      </c>
+      <c r="O8">
+        <v>42</v>
+      </c>
+      <c r="P8">
+        <v>1469151</v>
+      </c>
+      <c r="Q8">
+        <v>0.97819234784646603</v>
+      </c>
+      <c r="R8">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>1501906</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>168</v>
+      </c>
+      <c r="E9">
+        <v>123908</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>776095</v>
+      </c>
+      <c r="H9">
+        <v>0.51674006229417802</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>1129562</v>
+      </c>
+      <c r="K9">
+        <v>0.75208568312530799</v>
+      </c>
+      <c r="L9">
+        <v>17</v>
+      </c>
+      <c r="M9">
+        <v>1423386</v>
+      </c>
+      <c r="N9">
+        <v>0.94771976408643399</v>
+      </c>
+      <c r="O9">
+        <v>42</v>
+      </c>
+      <c r="P9">
+        <v>1470073</v>
+      </c>
+      <c r="Q9">
+        <v>0.97880493186657402</v>
+      </c>
+      <c r="R9">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>1501908</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>168</v>
+      </c>
+      <c r="E10">
+        <v>123908</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>776095</v>
+      </c>
+      <c r="H10">
+        <v>0.51673937418270599</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>1129562</v>
+      </c>
+      <c r="K10">
+        <v>0.75208468161831399</v>
+      </c>
+      <c r="L10">
+        <v>17</v>
+      </c>
+      <c r="M10">
+        <v>1423386</v>
+      </c>
+      <c r="N10">
+        <v>0.947718502065372</v>
+      </c>
+      <c r="O10">
+        <v>42</v>
+      </c>
+      <c r="P10">
+        <v>1470073</v>
+      </c>
+      <c r="Q10">
+        <v>0.978803628451276</v>
+      </c>
+      <c r="R10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>1516462</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>14554</v>
+      </c>
+      <c r="D11">
+        <v>190</v>
+      </c>
+      <c r="E11">
+        <v>123908</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>906041</v>
+      </c>
+      <c r="H11">
+        <v>0.59747029599159096</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>1175562</v>
+      </c>
+      <c r="K11">
+        <v>0.77520043364093505</v>
+      </c>
+      <c r="L11">
+        <v>19</v>
+      </c>
+      <c r="M11">
+        <v>1436073</v>
+      </c>
+      <c r="N11">
+        <v>0.94698911017882403</v>
+      </c>
+      <c r="O11">
+        <v>48</v>
+      </c>
+      <c r="P11">
+        <v>1483073</v>
+      </c>
+      <c r="Q11">
+        <v>0.97798230354601701</v>
+      </c>
+      <c r="R11">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>1516564</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="D12">
+        <v>192</v>
+      </c>
+      <c r="E12">
+        <v>123908</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>905949</v>
+      </c>
+      <c r="H12">
+        <v>0.59736944830551097</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>1175470</v>
+      </c>
+      <c r="K12">
+        <v>0.77508763230565902</v>
+      </c>
+      <c r="L12">
+        <v>19</v>
+      </c>
+      <c r="M12">
+        <v>1435981</v>
+      </c>
+      <c r="N12">
+        <v>0.94686475480098398</v>
+      </c>
+      <c r="O12">
+        <v>48</v>
+      </c>
+      <c r="P12">
+        <v>1483981</v>
+      </c>
+      <c r="Q12">
+        <v>0.97851524894432396</v>
+      </c>
+      <c r="R12">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>2009278</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>492714</v>
+      </c>
+      <c r="D13">
+        <v>205</v>
+      </c>
+      <c r="E13">
+        <v>143508</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>1062463</v>
+      </c>
+      <c r="H13">
+        <v>0.52877849655448295</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>1508666</v>
+      </c>
+      <c r="K13">
+        <v>0.75084980774188503</v>
+      </c>
+      <c r="L13">
+        <v>21</v>
+      </c>
+      <c r="M13">
+        <v>1918382</v>
+      </c>
+      <c r="N13">
+        <v>0.9547618597327</v>
+      </c>
+      <c r="O13">
+        <v>51</v>
+      </c>
+      <c r="P13">
+        <v>1974569</v>
+      </c>
+      <c r="Q13">
+        <v>0.98272563577563599</v>
+      </c>
+      <c r="R13">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>2028880</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>19602</v>
+      </c>
+      <c r="D14">
+        <v>206</v>
+      </c>
+      <c r="E14">
+        <v>143508</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>1062463</v>
+      </c>
+      <c r="H14">
+        <v>0.52366970939631696</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>1508666</v>
+      </c>
+      <c r="K14">
+        <v>0.74359548125073904</v>
+      </c>
+      <c r="L14">
+        <v>21</v>
+      </c>
+      <c r="M14">
+        <v>1937982</v>
+      </c>
+      <c r="N14">
+        <v>0.95519794172154004</v>
+      </c>
+      <c r="O14">
+        <v>52</v>
+      </c>
+      <c r="P14">
+        <v>1993169</v>
+      </c>
+      <c r="Q14">
+        <v>0.98239866330192005</v>
+      </c>
+      <c r="R14">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>2048482</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>19602</v>
+      </c>
+      <c r="D15">
+        <v>206</v>
+      </c>
+      <c r="E15">
+        <v>143508</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>1062463</v>
+      </c>
+      <c r="H15">
+        <v>0.51865869458457503</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>1513844</v>
+      </c>
+      <c r="K15">
+        <v>0.73900771400480902</v>
+      </c>
+      <c r="L15">
+        <v>21</v>
+      </c>
+      <c r="M15">
+        <v>1957580</v>
+      </c>
+      <c r="N15">
+        <v>0.95562470160831203</v>
+      </c>
+      <c r="O15">
+        <v>52</v>
+      </c>
+      <c r="P15">
+        <v>2012767</v>
+      </c>
+      <c r="Q15">
+        <v>0.98256513847815097</v>
+      </c>
+      <c r="R15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>2068084</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>19602</v>
+      </c>
+      <c r="D16">
+        <v>208</v>
+      </c>
+      <c r="E16">
+        <v>143508</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>1062463</v>
+      </c>
+      <c r="H16">
+        <v>0.51374267196110002</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>1513839</v>
+      </c>
+      <c r="K16">
+        <v>0.73200073111150199</v>
+      </c>
+      <c r="L16">
+        <v>21</v>
+      </c>
+      <c r="M16">
+        <v>1974675</v>
+      </c>
+      <c r="N16">
+        <v>0.95483307254444205</v>
+      </c>
+      <c r="O16">
+        <v>52</v>
+      </c>
+      <c r="P16">
+        <v>2032362</v>
+      </c>
+      <c r="Q16">
+        <v>0.982727007220209</v>
+      </c>
+      <c r="R16">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>2087686</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>19602</v>
+      </c>
+      <c r="D17">
+        <v>209</v>
+      </c>
+      <c r="E17">
+        <v>143508</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>1062463</v>
+      </c>
+      <c r="H17">
+        <v>0.50891896578316798</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>1513839</v>
+      </c>
+      <c r="K17">
+        <v>0.725127725146406</v>
+      </c>
+      <c r="L17">
+        <v>21</v>
+      </c>
+      <c r="M17">
+        <v>1991775</v>
+      </c>
+      <c r="N17">
+        <v>0.95405870423042505</v>
+      </c>
+      <c r="O17">
+        <v>52</v>
+      </c>
+      <c r="P17">
+        <v>2051962</v>
+      </c>
+      <c r="Q17">
+        <v>0.98288823127615899</v>
+      </c>
+      <c r="R17">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18">
+        <v>2094706</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>7020</v>
+      </c>
+      <c r="D18">
+        <v>219</v>
+      </c>
+      <c r="E18">
+        <v>143508</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>1127464</v>
+      </c>
+      <c r="H18">
+        <v>0.53824450782114497</v>
+      </c>
+      <c r="I18">
+        <v>11</v>
+      </c>
+      <c r="J18">
+        <v>1542331</v>
+      </c>
+      <c r="K18">
+        <v>0.73629950933448396</v>
+      </c>
+      <c r="L18">
+        <v>22</v>
+      </c>
+      <c r="M18">
+        <v>1999260</v>
+      </c>
+      <c r="N18">
+        <v>0.95443465574643804</v>
+      </c>
+      <c r="O18">
+        <v>55</v>
+      </c>
+      <c r="P18">
+        <v>2058447</v>
+      </c>
+      <c r="Q18">
+        <v>0.98269017227238498</v>
+      </c>
+      <c r="R18">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>2133912</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>39206</v>
+      </c>
+      <c r="D19">
+        <v>223</v>
+      </c>
+      <c r="E19">
+        <v>143508</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>1127464</v>
+      </c>
+      <c r="H19">
+        <v>0.52835543358863901</v>
+      </c>
+      <c r="I19">
+        <v>11</v>
+      </c>
+      <c r="J19">
+        <v>1542331</v>
+      </c>
+      <c r="K19">
+        <v>0.72277160445229205</v>
+      </c>
+      <c r="L19">
+        <v>22</v>
+      </c>
+      <c r="M19">
+        <v>2035851</v>
+      </c>
+      <c r="N19">
+        <v>0.95404637117181901</v>
+      </c>
+      <c r="O19">
+        <v>56</v>
+      </c>
+      <c r="P19">
+        <v>2097538</v>
+      </c>
+      <c r="Q19">
+        <v>0.98295431114310206</v>
+      </c>
+      <c r="R19">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>2203484</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>69572</v>
+      </c>
+      <c r="D20">
+        <v>257</v>
+      </c>
+      <c r="E20">
+        <v>143456</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>1220090</v>
+      </c>
+      <c r="H20">
+        <v>0.55370948915444795</v>
+      </c>
+      <c r="I20">
+        <v>13</v>
+      </c>
+      <c r="J20">
+        <v>1661044</v>
+      </c>
+      <c r="K20">
+        <v>0.75382621339660205</v>
+      </c>
+      <c r="L20">
+        <v>26</v>
+      </c>
+      <c r="M20">
+        <v>2101576</v>
+      </c>
+      <c r="N20">
+        <v>0.95375142274688596</v>
+      </c>
+      <c r="O20">
+        <v>64</v>
+      </c>
+      <c r="P20">
+        <v>2168761</v>
+      </c>
+      <c r="Q20">
+        <v>0.98424177348235797</v>
+      </c>
+      <c r="R20">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>2222520</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>19036</v>
+      </c>
+      <c r="D21">
+        <v>272</v>
+      </c>
+      <c r="E21">
+        <v>143456</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>1261690</v>
+      </c>
+      <c r="H21">
+        <v>0.56768443028634097</v>
+      </c>
+      <c r="I21">
+        <v>14</v>
+      </c>
+      <c r="J21">
+        <v>1687044</v>
+      </c>
+      <c r="K21">
+        <v>0.75906808487662603</v>
+      </c>
+      <c r="L21">
+        <v>27</v>
+      </c>
+      <c r="M21">
+        <v>2116064</v>
+      </c>
+      <c r="N21">
+        <v>0.95210121843672901</v>
+      </c>
+      <c r="O21">
+        <v>68</v>
+      </c>
+      <c r="P21">
+        <v>2184261</v>
+      </c>
+      <c r="Q21">
+        <v>0.98278575670860102</v>
+      </c>
+      <c r="R21">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22">
+        <v>2228530</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>6010</v>
+      </c>
+      <c r="D22">
+        <v>282</v>
+      </c>
+      <c r="E22">
+        <v>143466</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>1262124</v>
+      </c>
+      <c r="H22">
+        <v>0.56634822057589496</v>
+      </c>
+      <c r="I22">
+        <v>14</v>
+      </c>
+      <c r="J22">
+        <v>1708071</v>
+      </c>
+      <c r="K22">
+        <v>0.76645636361188696</v>
+      </c>
+      <c r="L22">
+        <v>28</v>
+      </c>
+      <c r="M22">
+        <v>2121678</v>
+      </c>
+      <c r="N22">
+        <v>0.95205269841554696</v>
+      </c>
+      <c r="O22">
+        <v>71</v>
+      </c>
+      <c r="P22">
+        <v>2191561</v>
+      </c>
+      <c r="Q22">
+        <v>0.98341103776929095</v>
+      </c>
+      <c r="R22">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>2234052</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>5522</v>
+      </c>
+      <c r="D23">
+        <v>292</v>
+      </c>
+      <c r="E23">
+        <v>143466</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>1302475</v>
+      </c>
+      <c r="H23">
+        <v>0.58301015374753995</v>
+      </c>
+      <c r="I23">
+        <v>15</v>
+      </c>
+      <c r="J23">
+        <v>1727552</v>
+      </c>
+      <c r="K23">
+        <v>0.77328191107458499</v>
+      </c>
+      <c r="L23">
+        <v>29</v>
+      </c>
+      <c r="M23">
+        <v>2126986</v>
+      </c>
+      <c r="N23">
+        <v>0.95207542170012105</v>
+      </c>
+      <c r="O23">
+        <v>73</v>
+      </c>
+      <c r="P23">
+        <v>2198201</v>
+      </c>
+      <c r="Q23">
+        <v>0.98395247738190506</v>
+      </c>
+      <c r="R23">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24">
+        <v>2250076</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>16024</v>
+      </c>
+      <c r="D24">
+        <v>301</v>
+      </c>
+      <c r="E24">
+        <v>143466</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>1302475</v>
+      </c>
+      <c r="H24">
+        <v>0.57885822523328101</v>
+      </c>
+      <c r="I24">
+        <v>15</v>
+      </c>
+      <c r="J24">
+        <v>1747152</v>
+      </c>
+      <c r="K24">
+        <v>0.776485772036144</v>
+      </c>
+      <c r="L24">
+        <v>30</v>
+      </c>
+      <c r="M24">
+        <v>2138997</v>
+      </c>
+      <c r="N24">
+        <v>0.95063322305557596</v>
+      </c>
+      <c r="O24">
+        <v>75</v>
+      </c>
+      <c r="P24">
+        <v>2212712</v>
+      </c>
+      <c r="Q24">
+        <v>0.98339433868011505</v>
+      </c>
+      <c r="R24">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <v>3073408</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>823332</v>
+      </c>
+      <c r="D25">
+        <v>305</v>
+      </c>
+      <c r="E25">
+        <v>163066</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>1554712</v>
+      </c>
+      <c r="H25">
+        <v>0.50585929365707305</v>
+      </c>
+      <c r="I25">
+        <v>15</v>
+      </c>
+      <c r="J25">
+        <v>2247850</v>
+      </c>
+      <c r="K25">
+        <v>0.73138678626462805</v>
+      </c>
+      <c r="L25">
+        <v>31</v>
+      </c>
+      <c r="M25">
+        <v>2950321</v>
+      </c>
+      <c r="N25">
+        <v>0.95995097299154497</v>
+      </c>
+      <c r="O25">
+        <v>76</v>
+      </c>
+      <c r="P25">
+        <v>3032115</v>
+      </c>
+      <c r="Q25">
+        <v>0.98656442620049101</v>
+      </c>
+      <c r="R25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26">
+        <v>3073910</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>502</v>
+      </c>
+      <c r="D26">
+        <v>307</v>
+      </c>
+      <c r="E26">
+        <v>163066</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>1554712</v>
+      </c>
+      <c r="H26">
+        <v>0.50577668181566804</v>
+      </c>
+      <c r="I26">
+        <v>15</v>
+      </c>
+      <c r="J26">
+        <v>2247850</v>
+      </c>
+      <c r="K26">
+        <v>0.73126734354616696</v>
+      </c>
+      <c r="L26">
+        <v>31</v>
+      </c>
+      <c r="M26">
+        <v>2952269</v>
+      </c>
+      <c r="N26">
+        <v>0.96042792404461996</v>
+      </c>
+      <c r="O26">
+        <v>77</v>
+      </c>
+      <c r="P26">
+        <v>3033062</v>
+      </c>
+      <c r="Q26">
+        <v>0.98671138712584205</v>
+      </c>
+      <c r="R26">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>3145563</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>71653</v>
+      </c>
+      <c r="D27">
+        <v>325</v>
+      </c>
+      <c r="E27">
+        <v>163066</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>1613759</v>
+      </c>
+      <c r="H27">
+        <v>0.51302707973103701</v>
+      </c>
+      <c r="I27">
+        <v>16</v>
+      </c>
+      <c r="J27">
+        <v>2334286</v>
+      </c>
+      <c r="K27">
+        <v>0.74208845920428201</v>
+      </c>
+      <c r="L27">
+        <v>33</v>
+      </c>
+      <c r="M27">
+        <v>3021537</v>
+      </c>
+      <c r="N27">
+        <v>0.96057112828450697</v>
+      </c>
+      <c r="O27">
+        <v>81</v>
+      </c>
+      <c r="P27">
+        <v>3106021</v>
+      </c>
+      <c r="Q27">
+        <v>0.98742927736624497</v>
+      </c>
+      <c r="R27">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>3188783</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>43220</v>
+      </c>
+      <c r="D28">
+        <v>330</v>
+      </c>
+      <c r="E28">
+        <v>163066</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>1672423</v>
+      </c>
+      <c r="H28">
+        <v>0.52447062092340502</v>
+      </c>
+      <c r="I28">
+        <v>17</v>
+      </c>
+      <c r="J28">
+        <v>2334286</v>
+      </c>
+      <c r="K28">
+        <v>0.73203037020706596</v>
+      </c>
+      <c r="L28">
+        <v>33</v>
+      </c>
+      <c r="M28">
+        <v>3064132</v>
+      </c>
+      <c r="N28">
+        <v>0.96090953821567604</v>
+      </c>
+      <c r="O28">
+        <v>83</v>
+      </c>
+      <c r="P28">
+        <v>3149227</v>
+      </c>
+      <c r="Q28">
+        <v>0.98759526753623506</v>
+      </c>
+      <c r="R28">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29">
+        <v>3194789</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>6006</v>
+      </c>
+      <c r="D29">
+        <v>330</v>
+      </c>
+      <c r="E29">
+        <v>163066</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <v>1672423</v>
+      </c>
+      <c r="H29">
+        <v>0.523484649533975</v>
+      </c>
+      <c r="I29">
+        <v>17</v>
+      </c>
+      <c r="J29">
+        <v>2334291</v>
+      </c>
+      <c r="K29">
+        <v>0.73065576474690497</v>
+      </c>
+      <c r="L29">
+        <v>33</v>
+      </c>
+      <c r="M29">
+        <v>3069622</v>
+      </c>
+      <c r="N29">
+        <v>0.96082151278222105</v>
+      </c>
+      <c r="O29">
+        <v>83</v>
+      </c>
+      <c r="P29">
+        <v>3154732</v>
+      </c>
+      <c r="Q29">
+        <v>0.98746176977571898</v>
+      </c>
+      <c r="R29">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30">
+        <v>4249717</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>1054928</v>
+      </c>
+      <c r="D30">
+        <v>341</v>
+      </c>
+      <c r="E30">
+        <v>182666</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>1968923</v>
+      </c>
+      <c r="H30">
+        <v>0.46330685078559303</v>
+      </c>
+      <c r="I30">
+        <v>17</v>
+      </c>
+      <c r="J30">
+        <v>2972110</v>
+      </c>
+      <c r="K30">
+        <v>0.69936656958569199</v>
+      </c>
+      <c r="L30">
+        <v>34</v>
+      </c>
+      <c r="M30">
+        <v>4106488</v>
+      </c>
+      <c r="N30">
+        <v>0.96629681458788896</v>
+      </c>
+      <c r="O30">
+        <v>85</v>
+      </c>
+      <c r="P30">
+        <v>4206017</v>
+      </c>
+      <c r="Q30">
+        <v>0.98971696232949102</v>
+      </c>
+      <c r="R30">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31">
+        <v>4312723</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>63006</v>
+      </c>
+      <c r="D31">
+        <v>344</v>
+      </c>
+      <c r="E31">
+        <v>182666</v>
+      </c>
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <v>1971423</v>
+      </c>
+      <c r="H31">
+        <v>0.45711792758310699</v>
+      </c>
+      <c r="I31">
+        <v>17</v>
+      </c>
+      <c r="J31">
+        <v>2984401</v>
+      </c>
+      <c r="K31">
+        <v>0.69199923111222295</v>
+      </c>
+      <c r="L31">
+        <v>34</v>
+      </c>
+      <c r="M31">
+        <v>4169078</v>
+      </c>
+      <c r="N31">
+        <v>0.96669273681615997</v>
+      </c>
+      <c r="O31">
+        <v>86</v>
+      </c>
+      <c r="P31">
+        <v>4268611</v>
+      </c>
+      <c r="Q31">
+        <v>0.98977165934375999</v>
+      </c>
+      <c r="R31">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32">
+        <v>4370337</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>57614</v>
+      </c>
+      <c r="D32">
+        <v>349</v>
+      </c>
+      <c r="E32">
+        <v>182666</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <v>2005923</v>
+      </c>
+      <c r="H32">
+        <v>0.45898588598545098</v>
+      </c>
+      <c r="I32">
+        <v>17</v>
+      </c>
+      <c r="J32">
+        <v>3063681</v>
+      </c>
+      <c r="K32">
+        <v>0.70101710691875696</v>
+      </c>
+      <c r="L32">
+        <v>35</v>
+      </c>
+      <c r="M32">
+        <v>4218667</v>
+      </c>
+      <c r="N32">
+        <v>0.96529558246881098</v>
+      </c>
+      <c r="O32">
+        <v>87</v>
+      </c>
+      <c r="P32">
+        <v>4324717</v>
+      </c>
+      <c r="Q32">
+        <v>0.98956144571917404</v>
+      </c>
+      <c r="R32">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33">
+        <v>4451373</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>81036</v>
+      </c>
+      <c r="D33">
+        <v>354</v>
+      </c>
+      <c r="E33">
+        <v>184666</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>2083650</v>
+      </c>
+      <c r="H33">
+        <v>0.46809153041095403</v>
+      </c>
+      <c r="I33">
+        <v>18</v>
+      </c>
+      <c r="J33">
+        <v>3078064</v>
+      </c>
+      <c r="K33">
+        <v>0.69148642452564602</v>
+      </c>
+      <c r="L33">
+        <v>35</v>
+      </c>
+      <c r="M33">
+        <v>4293148</v>
+      </c>
+      <c r="N33">
+        <v>0.96445478732067602</v>
+      </c>
+      <c r="O33">
+        <v>89</v>
+      </c>
+      <c r="P33">
+        <v>4405220</v>
+      </c>
+      <c r="Q33">
+        <v>0.989631738342304</v>
+      </c>
+      <c r="R33">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34">
+        <v>4489181</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>37808</v>
+      </c>
+      <c r="D34">
+        <v>361</v>
+      </c>
+      <c r="E34">
+        <v>189666</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <v>2094603</v>
+      </c>
+      <c r="H34">
+        <v>0.46658911725769098</v>
+      </c>
+      <c r="I34">
+        <v>18</v>
+      </c>
+      <c r="J34">
+        <v>3155715</v>
+      </c>
+      <c r="K34">
+        <v>0.70296007222698298</v>
+      </c>
+      <c r="L34">
+        <v>36</v>
+      </c>
+      <c r="M34">
+        <v>4330341</v>
+      </c>
+      <c r="N34">
+        <v>0.96461715399757697</v>
+      </c>
+      <c r="O34">
+        <v>90</v>
+      </c>
+      <c r="P34">
+        <v>4443835</v>
+      </c>
+      <c r="Q34">
+        <v>0.98989882564325204</v>
+      </c>
+      <c r="R34">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35">
+        <v>4528692</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>39511</v>
+      </c>
+      <c r="D35">
+        <v>368</v>
+      </c>
+      <c r="E35">
+        <v>194342</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35">
+        <v>2103539</v>
+      </c>
+      <c r="H35">
+        <v>0.46449151322280202</v>
+      </c>
+      <c r="I35">
+        <v>18</v>
+      </c>
+      <c r="J35">
+        <v>3211743</v>
+      </c>
+      <c r="K35">
+        <v>0.70919881502208504</v>
+      </c>
+      <c r="L35">
+        <v>37</v>
+      </c>
+      <c r="M35">
+        <v>4377800</v>
+      </c>
+      <c r="N35">
+        <v>0.96668088710824196</v>
+      </c>
+      <c r="O35">
+        <v>92</v>
+      </c>
+      <c r="P35">
+        <v>4485366</v>
+      </c>
+      <c r="Q35">
+        <v>0.99043299919711902</v>
+      </c>
+      <c r="R35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <v>4528692</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>340</v>
+      </c>
+      <c r="E36">
+        <v>194342</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36">
+        <v>2030853</v>
+      </c>
+      <c r="H36">
+        <v>0.44844140427302098</v>
+      </c>
+      <c r="I36">
+        <v>17</v>
+      </c>
+      <c r="J36">
+        <v>3055552</v>
+      </c>
+      <c r="K36">
+        <v>0.67470960710068095</v>
+      </c>
+      <c r="L36">
+        <v>34</v>
+      </c>
+      <c r="M36">
+        <v>4345800</v>
+      </c>
+      <c r="N36">
+        <v>0.95961482918246499</v>
+      </c>
+      <c r="O36">
+        <v>85</v>
+      </c>
+      <c r="P36">
+        <v>4473095</v>
+      </c>
+      <c r="Q36">
+        <v>0.98772338679689398</v>
+      </c>
+      <c r="R36">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>4528692</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>340</v>
+      </c>
+      <c r="E37">
+        <v>194342</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37">
+        <v>2030853</v>
+      </c>
+      <c r="H37">
+        <v>0.44844140427302098</v>
+      </c>
+      <c r="I37">
+        <v>17</v>
+      </c>
+      <c r="J37">
+        <v>3055552</v>
+      </c>
+      <c r="K37">
+        <v>0.67470960710068095</v>
+      </c>
+      <c r="L37">
+        <v>34</v>
+      </c>
+      <c r="M37">
+        <v>4345800</v>
+      </c>
+      <c r="N37">
+        <v>0.95961482918246499</v>
+      </c>
+      <c r="O37">
+        <v>85</v>
+      </c>
+      <c r="P37">
+        <v>4473095</v>
+      </c>
+      <c r="Q37">
+        <v>0.98772338679689398</v>
+      </c>
+      <c r="R37">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38">
+        <v>5595214</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>1066522</v>
+      </c>
+      <c r="D38">
+        <v>347</v>
+      </c>
+      <c r="E38">
+        <v>213942</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>2355314</v>
+      </c>
+      <c r="H38">
+        <v>0.42095154894879799</v>
+      </c>
+      <c r="I38">
+        <v>17</v>
+      </c>
+      <c r="J38">
+        <v>3734836</v>
+      </c>
+      <c r="K38">
+        <v>0.66750547878955102</v>
+      </c>
+      <c r="L38">
+        <v>35</v>
+      </c>
+      <c r="M38">
+        <v>5409271</v>
+      </c>
+      <c r="N38">
+        <v>0.96676749093064096</v>
+      </c>
+      <c r="O38">
+        <v>87</v>
+      </c>
+      <c r="P38">
+        <v>5541068</v>
+      </c>
+      <c r="Q38">
+        <v>0.990322800879465</v>
+      </c>
+      <c r="R38">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39">
+        <v>5647002</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>51788</v>
+      </c>
+      <c r="D39">
+        <v>356</v>
+      </c>
+      <c r="E39">
+        <v>213942</v>
+      </c>
+      <c r="F39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39">
+        <v>2445774</v>
+      </c>
+      <c r="H39">
+        <v>0.43311017067109198</v>
+      </c>
+      <c r="I39">
+        <v>18</v>
+      </c>
+      <c r="J39">
+        <v>3820963</v>
+      </c>
+      <c r="K39">
+        <v>0.67663567322979501</v>
+      </c>
+      <c r="L39">
+        <v>36</v>
+      </c>
+      <c r="M39">
+        <v>5459767</v>
+      </c>
+      <c r="N39">
+        <v>0.96684346844573399</v>
+      </c>
+      <c r="O39">
+        <v>89</v>
+      </c>
+      <c r="P39">
+        <v>5593232</v>
+      </c>
+      <c r="Q39">
+        <v>0.99047813335288304</v>
+      </c>
+      <c r="R39">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>5649512</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>2510</v>
+      </c>
+      <c r="D40">
+        <v>357</v>
+      </c>
+      <c r="E40">
+        <v>213942</v>
+      </c>
+      <c r="F40" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40">
+        <v>2445774</v>
+      </c>
+      <c r="H40">
+        <v>0.43291774581592102</v>
+      </c>
+      <c r="I40">
+        <v>18</v>
+      </c>
+      <c r="J40">
+        <v>3820963</v>
+      </c>
+      <c r="K40">
+        <v>0.67633505336390098</v>
+      </c>
+      <c r="L40">
+        <v>36</v>
+      </c>
+      <c r="M40">
+        <v>5459767</v>
+      </c>
+      <c r="N40">
+        <v>0.96641391327250903</v>
+      </c>
+      <c r="O40">
+        <v>89</v>
+      </c>
+      <c r="P40">
+        <v>5595232</v>
+      </c>
+      <c r="Q40">
+        <v>0.99039209050268395</v>
+      </c>
+      <c r="R40">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41">
+        <v>5649512</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>359</v>
+      </c>
+      <c r="E41">
+        <v>213942</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41">
+        <v>2445758</v>
+      </c>
+      <c r="H41">
+        <v>0.43291491371290097</v>
+      </c>
+      <c r="I41">
+        <v>18</v>
+      </c>
+      <c r="J41">
+        <v>3820947</v>
+      </c>
+      <c r="K41">
+        <v>0.67633222126088</v>
+      </c>
+      <c r="L41">
+        <v>36</v>
+      </c>
+      <c r="M41">
+        <v>5463749</v>
+      </c>
+      <c r="N41">
+        <v>0.96711875291175498</v>
+      </c>
+      <c r="O41">
+        <v>90</v>
+      </c>
+      <c r="P41">
+        <v>5595214</v>
+      </c>
+      <c r="Q41">
+        <v>0.99038890438678595</v>
+      </c>
+      <c r="R41">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E3:E40">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="7"/>
+        <color theme="5"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D40">
+    <cfRule type="dataBar" priority="36">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E53CF63B-C6A2-437F-BD74-DE8E2A2B0646}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H40">
+    <cfRule type="cellIs" dxfId="7" priority="32" operator="greaterThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K40">
+    <cfRule type="cellIs" dxfId="6" priority="31" operator="greaterThan">
+      <formula>0.75</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N40">
+    <cfRule type="cellIs" dxfId="5" priority="30" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q40">
+    <cfRule type="cellIs" dxfId="4" priority="29" operator="greaterThan">
+      <formula>0.9846</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L40">
+    <cfRule type="dataBar" priority="28">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D446B47B-4955-4A6C-B114-A20B91161404}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I40">
+    <cfRule type="dataBar" priority="27">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CF7B9F07-76DE-462E-A1DC-65EFC5B61DFE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O40">
+    <cfRule type="dataBar" priority="26">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0CCDC196-9CF6-4096-85CF-9D4543E751E2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3:R40">
+    <cfRule type="dataBar" priority="25">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{80EFE7A8-677F-4AC0-8AB9-5998B061BF05}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B40">
+    <cfRule type="dataBar" priority="24">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5B746880-6434-4DD6-9EAE-773A44FD35E0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G40">
+    <cfRule type="dataBar" priority="23">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5442310D-4C89-4D10-9D5A-0002C01C4CE8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J40">
+    <cfRule type="dataBar" priority="22">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{814EFA5D-D5BF-4A8F-8D34-0F80356FA4BA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M40">
+    <cfRule type="dataBar" priority="21">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{686619B8-E037-4B4B-BDC2-81B161207F8D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P40">
+    <cfRule type="dataBar" priority="20">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{744EA3D8-FEE4-4A4E-9FFB-EBB589173F6B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="7"/>
+        <color theme="5"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E7AE562C-9B5A-44C7-A4F9-9476122D7774}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="greaterThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K41">
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="greaterThan">
+      <formula>0.75</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N41">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q41">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="greaterThan">
+      <formula>0.9846</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L41">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{88622B2B-6C49-446A-BB26-E76703ABC9AA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2863C4BC-65C6-4A8D-8A89-F10A662A9D2A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O41">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{577A36BE-E1BC-4BBB-87D0-A7A18E9688BE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R41">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8DA01343-6381-4BEC-A1D3-802092109C88}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{47E24241-80E4-44ED-8AE3-7F08D7F785AE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FFD06FDF-39C0-4D80-AC91-FFC6DCC9C0C5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0A0244AC-0887-4ABF-ABF7-CDD3673951EA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M41">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C9C43021-08C6-4D5C-B602-E8DEDF5D5DB6}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P41">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C356A110-F2B1-49E8-AA1E-2511A3421D1E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E53CF63B-C6A2-437F-BD74-DE8E2A2B0646}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D3:D40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D446B47B-4955-4A6C-B114-A20B91161404}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L3:L40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CF7B9F07-76DE-462E-A1DC-65EFC5B61DFE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I3:I40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0CCDC196-9CF6-4096-85CF-9D4543E751E2}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O3:O40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{80EFE7A8-677F-4AC0-8AB9-5998B061BF05}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>R3:R40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5B746880-6434-4DD6-9EAE-773A44FD35E0}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B3:B40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5442310D-4C89-4D10-9D5A-0002C01C4CE8}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G3:G40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{814EFA5D-D5BF-4A8F-8D34-0F80356FA4BA}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J3:J40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{686619B8-E037-4B4B-BDC2-81B161207F8D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M3:M40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{744EA3D8-FEE4-4A4E-9FFB-EBB589173F6B}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P3:P40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E7AE562C-9B5A-44C7-A4F9-9476122D7774}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{88622B2B-6C49-446A-BB26-E76703ABC9AA}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2863C4BC-65C6-4A8D-8A89-F10A662A9D2A}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{577A36BE-E1BC-4BBB-87D0-A7A18E9688BE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8DA01343-6381-4BEC-A1D3-802092109C88}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>R41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{47E24241-80E4-44ED-8AE3-7F08D7F785AE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FFD06FDF-39C0-4D80-AC91-FFC6DCC9C0C5}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0A0244AC-0887-4ABF-ABF7-CDD3673951EA}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C9C43021-08C6-4D5C-B602-E8DEDF5D5DB6}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C356A110-F2B1-49E8-AA1E-2511A3421D1E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="33" id="{C30227DF-0633-4217-8D77-4CF5F898F9A8}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <x14:cfRule type="iconSet" priority="34" id="{217203F3-33B0-4CBC-8D87-B5C3D36154C6}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <x14:cfRule type="iconSet" priority="35" id="{65C86BD9-0948-4DCC-AE84-63E428155B39}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>C4:C41</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="108" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
@@ -3345,7 +6556,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R40">
+  <sortState ref="A3:R40">
     <sortCondition ref="A3:A40"/>
   </sortState>
   <mergeCells count="10">
@@ -3393,22 +6604,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H40">
-    <cfRule type="cellIs" dxfId="3" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K40">
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
       <formula>0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N40">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q40">
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
       <formula>0.9846</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added visualization jupyter notebook
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\Desktop\web\analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E2F675-CC06-4DCC-B58D-2F4395413E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="5415" yWindow="1605" windowWidth="19830" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="out" sheetId="2" r:id="rId1"/>
@@ -199,7 +205,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
@@ -775,9 +781,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -785,6 +788,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1258,23 +1264,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
@@ -1291,52 +1297,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="14" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14" t="s">
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="18"/>
-      <c r="F2" s="14"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
@@ -3642,22 +3648,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H40">
-    <cfRule type="cellIs" dxfId="7" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="32" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K40">
-    <cfRule type="cellIs" dxfId="6" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="31" operator="greaterThan">
       <formula>0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N40">
-    <cfRule type="cellIs" dxfId="5" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="30" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q40">
-    <cfRule type="cellIs" dxfId="4" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="29" operator="greaterThan">
       <formula>0.9846</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3820,22 +3826,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="cellIs" dxfId="3" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41">
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="greaterThan">
       <formula>0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q41">
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="greaterThan">
       <formula>0.9846</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4281,7 +4287,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView zoomScale="108" zoomScaleNormal="110" workbookViewId="0">
@@ -4307,52 +4313,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="14" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14" t="s">
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="18"/>
-      <c r="F2" s="14"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
@@ -6556,20 +6562,20 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:R40">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R40">
     <sortCondition ref="A3:A40"/>
   </sortState>
   <mergeCells count="10">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E40">
     <cfRule type="colorScale" priority="19">
@@ -6604,22 +6610,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H40">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K40">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="greaterThan">
       <formula>0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N40">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q40">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="greaterThan">
       <formula>0.9846</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>